<commit_message>
Cambio da "appuntamento" e "prestazione"
</commit_message>
<xml_diff>
--- a/Tabella Volumi.xlsx
+++ b/Tabella Volumi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\OneDrive\Desktop\uni\db\ClinicPrive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ClinicPrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FD4CDEA-E4AE-4D5C-AD53-8A94F61105D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BF9B08-B4BD-49A9-9B41-D639F4C94135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6A23761B-8802-44C7-9743-49F63CD26C83}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>Concetto</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Sala</t>
   </si>
   <si>
-    <t>Luogo</t>
-  </si>
-  <si>
     <t>Indirizzo</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>Persona</t>
   </si>
   <si>
-    <t xml:space="preserve">Proprietà </t>
-  </si>
-  <si>
     <t>Amministratore</t>
   </si>
   <si>
@@ -174,27 +168,9 @@
     <t>Patologia</t>
   </si>
   <si>
-    <t>Prescrizione Vecchia</t>
-  </si>
-  <si>
-    <t>Terapia Precedente</t>
-  </si>
-  <si>
-    <t>Inclusione T. Precedente</t>
-  </si>
-  <si>
     <t>Farmaco</t>
   </si>
   <si>
-    <t>Inclusione T. Medico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terapia Medico </t>
-  </si>
-  <si>
-    <t>Prescrizione Nuova</t>
-  </si>
-  <si>
     <t>Accoglienza</t>
   </si>
   <si>
@@ -202,6 +178,15 @@
   </si>
   <si>
     <t>Assistente</t>
+  </si>
+  <si>
+    <t>Terapia</t>
+  </si>
+  <si>
+    <t>Inclusione</t>
+  </si>
+  <si>
+    <t>Prescrizione</t>
   </si>
 </sst>
 </file>
@@ -225,7 +210,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -233,55 +218,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -297,10 +242,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86E48BF6-C6DA-4A6B-BCAB-21E05FC41A8D}" name="Table1" displayName="Table1" ref="B3:D54" totalsRowShown="0">
-  <autoFilter ref="B3:D54" xr:uid="{86E48BF6-C6DA-4A6B-BCAB-21E05FC41A8D}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:D54">
-    <sortCondition ref="C3:C54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86E48BF6-C6DA-4A6B-BCAB-21E05FC41A8D}" name="Table1" displayName="Table1" ref="B3:D49" totalsRowShown="0">
+  <autoFilter ref="B3:D49" xr:uid="{86E48BF6-C6DA-4A6B-BCAB-21E05FC41A8D}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:D49">
+    <sortCondition ref="C3:C49"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C1ECC5E7-41B7-4DA9-9C12-408A7DCA5E0B}" name="Concetto"/>
@@ -312,9 +261,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -352,7 +301,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -458,7 +407,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -600,7 +549,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -608,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D8D700-9028-4214-B429-937A99143D19}">
-  <dimension ref="B3:U54"/>
+  <dimension ref="B3:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -634,7 +583,7 @@
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -645,7 +594,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -656,7 +605,7 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -678,7 +627,7 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -700,7 +649,7 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -711,7 +660,7 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -733,7 +682,7 @@
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -744,7 +693,7 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -755,7 +704,7 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -766,7 +715,7 @@
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -777,7 +726,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -788,7 +737,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -799,7 +748,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -810,7 +759,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -832,7 +781,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -865,7 +814,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -876,330 +825,273 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
       </c>
       <c r="D26">
-        <v>7000</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
       </c>
       <c r="D27">
-        <v>12000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
       </c>
       <c r="D28">
-        <v>500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29">
-        <v>900</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D30">
-        <v>30000</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
         <v>13</v>
       </c>
       <c r="D31">
-        <v>7000</v>
+        <v>42500</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
         <v>42</v>
       </c>
-      <c r="C32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32">
+      <c r="C36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>12066</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38">
         <v>42500</v>
       </c>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39">
         <v>500</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D34">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40">
+        <v>18500</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44">
+        <v>19000</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45">
         <v>14000</v>
       </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B36" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38">
-        <v>12066</v>
-      </c>
-    </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39">
-        <v>42500</v>
-      </c>
-    </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B40" t="s">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46">
+        <v>165000</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
         <v>30</v>
       </c>
-      <c r="C40" t="s">
-        <v>13</v>
-      </c>
-      <c r="D40">
+      <c r="C47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47">
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41">
-        <v>10500</v>
-      </c>
-    </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
-        <v>48</v>
-      </c>
-      <c r="C42" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="S43" s="1"/>
-      <c r="T43" s="2"/>
-      <c r="U43" s="3"/>
-    </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
-        <v>37</v>
-      </c>
-      <c r="C44" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
-        <v>41</v>
-      </c>
-      <c r="C46" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46">
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
         <v>13</v>
       </c>
       <c r="D48">
-        <v>12000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C49" t="s">
         <v>13</v>
       </c>
       <c r="D49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B50" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B51" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51">
-        <v>165000</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B52" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" t="s">
-        <v>13</v>
-      </c>
-      <c r="D53">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B54" t="s">
-        <v>36</v>
-      </c>
-      <c r="C54" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54">
         <v>165000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>